<commit_message>
guizmo test with camera
</commit_message>
<xml_diff>
--- a/Sunshine_-_Production_Plan_Template.xlsx
+++ b/Sunshine_-_Production_Plan_Template.xlsx
@@ -25,7 +25,7 @@
   </definedNames>
   <calcPr calcId="152511"/>
   <pivotCaches>
-    <pivotCache cacheId="20" r:id="rId6"/>
+    <pivotCache cacheId="5" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext uri="GoogleSheetsCustomDataVersion1">
@@ -81,7 +81,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1285" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1309" uniqueCount="126">
   <si>
     <t>BACKLOG</t>
   </si>
@@ -454,6 +454,12 @@
   <si>
     <t>sy/yx</t>
   </si>
+  <si>
+    <t>Correcting Old scripts</t>
+  </si>
+  <si>
+    <t>Debug Old AI behaviour</t>
+  </si>
 </sst>
 </file>
 
@@ -672,7 +678,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="30">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1005,11 +1011,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFABABAB"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFABABAB"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFABABAB"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1130,27 +1156,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" pivotButton="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
@@ -1166,6 +1171,31 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" pivotButton="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="18" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1229,7 +1259,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Shuyu YIN" refreshedDate="43853.741858217596" refreshedVersion="5" recordCount="109">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Shuyu YIN" refreshedDate="43853.804906597223" refreshedVersion="5" recordCount="109">
   <cacheSource type="worksheet">
     <worksheetSource ref="B3:I112" sheet="Tech Backlog"/>
   </cacheSource>
@@ -1237,21 +1267,27 @@
     <cacheField name="Completion" numFmtId="0">
       <sharedItems count="3">
         <s v="Not Started"/>
+        <s v="In Progress"/>
         <s v="Done"/>
-        <s v="In Progress"/>
       </sharedItems>
     </cacheField>
     <cacheField name="Priority" numFmtId="0">
-      <sharedItems/>
+      <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="EPIC" numFmtId="0">
-      <sharedItems/>
+      <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Task" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+      <sharedItems containsBlank="1"/>
     </cacheField>
     <cacheField name="Owner" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+      <sharedItems containsBlank="1" count="7">
+        <s v="ym"/>
+        <s v="ym/yx"/>
+        <s v="br"/>
+        <s v="yx"/>
+        <s v="sy"/>
+        <s v="sy/yx"/>
         <m/>
       </sharedItems>
     </cacheField>
@@ -1259,11 +1295,15 @@
       <sharedItems/>
     </cacheField>
     <cacheField name="Estimation (h)" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1"/>
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="2" maxValue="24"/>
     </cacheField>
     <cacheField name="Planned Week" numFmtId="0">
-      <sharedItems containsNonDate="0" containsString="0" containsBlank="1" count="1">
+      <sharedItems containsString="0" containsBlank="1" containsNumber="1" containsInteger="1" minValue="3" maxValue="10" count="5">
+        <n v="6"/>
+        <n v="4"/>
+        <n v="3"/>
         <m/>
+        <n v="10"/>
       </sharedItems>
     </cacheField>
   </cacheFields>
@@ -1279,1105 +1319,1105 @@
 <pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="109">
   <r>
     <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Abilities"/>
-    <m/>
+    <s v="1 - Should Have"/>
+    <m/>
+    <s v="Batch Renderer"/>
     <x v="0"/>
     <s v="Code"/>
-    <m/>
+    <n v="10"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="1 - Should Have"/>
+    <m/>
+    <s v="Animation Component cleanup"/>
+    <x v="1"/>
+    <s v="Code"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="1 - Should Have"/>
+    <m/>
+    <s v="Shader for effects"/>
+    <x v="0"/>
+    <s v="Code"/>
+    <n v="12"/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="1 - Should Have"/>
+    <m/>
+    <s v="Fix Lua Scripting"/>
+    <x v="2"/>
+    <s v="Code"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="1 - Should Have"/>
+    <m/>
+    <s v="Animation system for editor"/>
+    <x v="3"/>
+    <s v="Code"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="1 - Should Have"/>
+    <m/>
+    <s v="Particle system"/>
+    <x v="4"/>
+    <s v="Code"/>
+    <n v="24"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="0 - Must Have"/>
+    <m/>
+    <s v="Fix | update Inspection"/>
+    <x v="5"/>
+    <s v="Code"/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="1 - Should Have"/>
+    <m/>
+    <s v="Camera system"/>
+    <x v="0"/>
+    <s v="Code"/>
+    <n v="6"/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <s v="Editor UI"/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <m/>
+    <m/>
+    <s v="Fix gizmo"/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="0 - Must Have"/>
+    <m/>
+    <s v="Fix Save of scene and prototype"/>
+    <x v="5"/>
+    <s v="Code"/>
+    <m/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="0 - Must Have"/>
+    <m/>
+    <s v="Fix Add Component crashes"/>
+    <x v="5"/>
+    <s v="Animation"/>
+    <n v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="0 - Must Have"/>
+    <m/>
+    <s v="Fix lose of swtiching of Graphic image"/>
+    <x v="5"/>
+    <s v="Animation"/>
+    <n v="5"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <s v="0 - Must Have"/>
+    <m/>
+    <s v="editer camera "/>
+    <x v="2"/>
+    <s v="Animation"/>
+    <n v="2"/>
+    <x v="2"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="1 - Should Have"/>
+    <m/>
+    <s v="polygon collider component"/>
+    <x v="4"/>
+    <s v="Animation"/>
+    <m/>
+    <x v="0"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="1 - Should Have"/>
+    <m/>
+    <s v="Audio Component"/>
+    <x v="4"/>
+    <s v="Animation"/>
+    <m/>
+    <x v="1"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <s v="1 - Should Have"/>
+    <m/>
+    <s v="Add on UI Component"/>
+    <x v="1"/>
+    <s v="Animation"/>
+    <n v="6"/>
     <x v="0"/>
   </r>
   <r>
     <x v="0"/>
     <s v="2 - Could Have"/>
-    <s v="Abilities"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Abilities"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Abilities"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Abilities"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Abilities"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Make Editor more user friendly"/>
+    <x v="5"/>
+    <s v="Animation"/>
+    <m/>
+    <x v="4"/>
   </r>
   <r>
     <x v="0"/>
     <s v="2 - Could Have"/>
-    <s v="Abilities"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Play in edtitor mode"/>
+    <x v="5"/>
+    <s v="Animation"/>
+    <m/>
+    <x v="4"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Abilities"/>
-    <m/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="6"/>
+    <s v="Animation"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
     <x v="0"/>
+    <m/>
+    <m/>
+    <m/>
+    <x v="6"/>
+    <s v="Animation"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="2"/>
+    <m/>
+    <s v="Character"/>
+    <m/>
+    <x v="6"/>
     <s v="Code"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="1"/>
-    <s v="0 - Must Have"/>
-    <s v="Camera"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Character"/>
+    <m/>
+    <x v="6"/>
+    <s v="3D Art"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Camera"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Character"/>
+    <m/>
+    <x v="6"/>
+    <s v="Animation"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Camera"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Character"/>
+    <m/>
+    <x v="6"/>
+    <s v="Animation"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="2 - Could Have"/>
+    <m/>
     <s v="Character"/>
     <m/>
-    <x v="0"/>
+    <x v="6"/>
     <s v="Animation"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
+    <m/>
     <s v="Character"/>
     <m/>
-    <x v="0"/>
+    <x v="6"/>
     <s v="Animation"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
+    <m/>
     <s v="Character"/>
     <m/>
-    <x v="0"/>
-    <s v="Animation"/>
-    <m/>
-    <x v="0"/>
+    <x v="6"/>
+    <s v="3D Art"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
+    <m/>
     <s v="Character"/>
     <m/>
-    <x v="0"/>
-    <s v="Animation"/>
-    <m/>
-    <x v="0"/>
+    <x v="6"/>
+    <s v="3D Art"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
+    <m/>
     <s v="Character"/>
     <m/>
-    <x v="0"/>
-    <s v="Animation"/>
-    <m/>
-    <x v="0"/>
+    <x v="6"/>
+    <s v="3D Art"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
+    <m/>
     <s v="Character"/>
     <m/>
-    <x v="0"/>
-    <s v="Animation"/>
-    <m/>
-    <x v="0"/>
+    <x v="6"/>
+    <s v="3D Art"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
+    <m/>
     <s v="Character"/>
     <m/>
-    <x v="0"/>
-    <s v="Animation"/>
-    <m/>
-    <x v="0"/>
+    <x v="6"/>
+    <s v="3D Art"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
+    <m/>
     <s v="Character"/>
     <m/>
-    <x v="0"/>
-    <s v="Animation"/>
-    <m/>
-    <x v="0"/>
+    <x v="6"/>
+    <s v="3D Art"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
+    <m/>
     <s v="Character"/>
     <m/>
-    <x v="0"/>
-    <s v="Animation"/>
-    <m/>
-    <x v="0"/>
+    <x v="6"/>
+    <s v="3D Art"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
+    <m/>
     <s v="Character"/>
     <m/>
+    <x v="6"/>
+    <s v="3D Art"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
     <x v="0"/>
+    <m/>
+    <s v="Character"/>
+    <m/>
+    <x v="6"/>
+    <s v="3D Art"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <s v="Character"/>
+    <m/>
+    <x v="6"/>
+    <s v="3D Art"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <s v="Character"/>
+    <m/>
+    <x v="6"/>
+    <s v="3D Art"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <s v="Character"/>
+    <m/>
+    <x v="6"/>
     <s v="Animation"/>
     <m/>
+    <x v="3"/>
+  </r>
+  <r>
     <x v="0"/>
+    <m/>
+    <s v="Character"/>
+    <m/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="1"/>
-    <s v="0 - Must Have"/>
-    <s v="Character"/>
-    <m/>
+    <m/>
+    <s v="Combat"/>
+    <m/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
     <x v="0"/>
+    <m/>
+    <s v="Combat"/>
+    <m/>
+    <x v="6"/>
     <s v="Code"/>
     <m/>
+    <x v="3"/>
+  </r>
+  <r>
     <x v="0"/>
+    <m/>
+    <s v="Combat"/>
+    <m/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <s v="Combat"/>
+    <m/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <s v="Enemy AI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <s v="Enemy AI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <s v="Enemy AI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <s v="Enemy AI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <s v="Enemy AI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <s v="Enemy AI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <m/>
+    <s v="Enemy AI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <s v="Enemy AI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <s v="Enemy AI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <s v="Enemy AI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="2"/>
-    <s v="0 - Must Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
-    <s v="3D Art"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Music"/>
+    <m/>
+    <x v="6"/>
+    <s v="Other"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <m/>
+    <s v="Music"/>
+    <m/>
+    <x v="6"/>
+    <s v="Other"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
-    <s v="Animation"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Music"/>
+    <m/>
+    <x v="6"/>
+    <s v="Other"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
-    <s v="Animation"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Music"/>
+    <m/>
+    <x v="6"/>
+    <s v="Other"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
-    <s v="Animation"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Music"/>
+    <m/>
+    <x v="6"/>
+    <s v="Other"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <m/>
+    <s v="Props"/>
+    <m/>
+    <x v="6"/>
+    <s v="3D Art"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
-    <s v="Animation"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Props"/>
+    <m/>
+    <x v="6"/>
+    <s v="3D Art"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Props"/>
+    <m/>
+    <x v="6"/>
     <s v="3D Art"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Props"/>
+    <m/>
+    <x v="6"/>
     <s v="3D Art"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Props"/>
+    <m/>
+    <x v="6"/>
     <s v="3D Art"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Props"/>
+    <m/>
+    <x v="6"/>
     <s v="3D Art"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Props"/>
+    <m/>
+    <x v="6"/>
     <s v="3D Art"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Props"/>
+    <m/>
+    <x v="6"/>
     <s v="3D Art"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Props"/>
+    <m/>
+    <x v="6"/>
     <s v="3D Art"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Props"/>
+    <m/>
+    <x v="6"/>
     <s v="3D Art"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Props"/>
+    <m/>
+    <x v="6"/>
     <s v="3D Art"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Props"/>
+    <m/>
+    <x v="6"/>
     <s v="3D Art"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Props"/>
+    <m/>
+    <x v="6"/>
     <s v="3D Art"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
-    <s v="Animation"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Props"/>
+    <m/>
+    <x v="6"/>
+    <s v="3D Art"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Character"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <s v="0 - Must Have"/>
-    <s v="Combat"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Props"/>
+    <m/>
+    <x v="6"/>
+    <s v="3D Art"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Combat"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Props"/>
+    <m/>
+    <x v="6"/>
+    <s v="3D Art"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Combat"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Puzzle"/>
+    <m/>
+    <x v="6"/>
     <s v="Code"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Combat"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Puzzle"/>
+    <m/>
+    <x v="6"/>
     <s v="Code"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Enemy AI"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Puzzle"/>
+    <m/>
+    <x v="6"/>
     <s v="Code"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="1"/>
+    <m/>
+    <s v="UI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Enemy AI"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="UI"/>
+    <m/>
+    <x v="6"/>
     <s v="Code"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Enemy AI"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="UI"/>
+    <m/>
+    <x v="6"/>
     <s v="Code"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Enemy AI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="UI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Other"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Enemy AI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="UI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Other"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Enemy AI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <s v="0 - Must Have"/>
-    <s v="Enemy AI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="UI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Other"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Enemy AI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="UI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Other"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Enemy AI"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="UI"/>
+    <m/>
+    <x v="6"/>
     <s v="Code"/>
     <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Enemy AI"/>
-    <m/>
+    <m/>
+    <s v="UI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
     <x v="0"/>
+    <m/>
+    <s v="UI"/>
+    <m/>
+    <x v="6"/>
     <s v="Code"/>
     <m/>
+    <x v="3"/>
+  </r>
+  <r>
     <x v="0"/>
+    <m/>
+    <s v="UI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Code"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <s v="UI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Other"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <s v="UI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Other"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <s v="UI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Other"/>
+    <m/>
+    <x v="3"/>
+  </r>
+  <r>
+    <x v="0"/>
+    <m/>
+    <s v="UI"/>
+    <m/>
+    <x v="6"/>
+    <s v="Other"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="1"/>
-    <s v="0 - Must Have"/>
-    <s v="Music"/>
-    <m/>
-    <x v="0"/>
-    <s v="Other"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <s v="0 - Must Have"/>
-    <s v="Music"/>
-    <m/>
-    <x v="0"/>
-    <s v="Other"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="World"/>
+    <m/>
+    <x v="6"/>
+    <s v="Level Design"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Music"/>
-    <m/>
-    <x v="0"/>
-    <s v="Other"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="World"/>
+    <m/>
+    <x v="6"/>
+    <s v="Level Design"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Music"/>
-    <m/>
-    <x v="0"/>
-    <s v="Other"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="World"/>
+    <m/>
+    <x v="6"/>
+    <s v="Level Design"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Music"/>
-    <m/>
-    <x v="0"/>
-    <s v="Other"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <s v="0 - Must Have"/>
-    <s v="Props"/>
-    <m/>
-    <x v="0"/>
-    <s v="3D Art"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="World"/>
+    <m/>
+    <x v="6"/>
+    <s v="Level Design"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Props"/>
-    <m/>
-    <x v="0"/>
-    <s v="3D Art"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="World"/>
+    <m/>
+    <x v="6"/>
+    <s v="Level Design"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Props"/>
-    <m/>
-    <x v="0"/>
-    <s v="3D Art"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="World"/>
+    <m/>
+    <x v="6"/>
+    <s v="Level Design"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Props"/>
-    <m/>
-    <x v="0"/>
-    <s v="3D Art"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="World"/>
+    <m/>
+    <x v="6"/>
+    <s v="Level Design"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Props"/>
-    <m/>
-    <x v="0"/>
-    <s v="3D Art"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="World"/>
+    <m/>
+    <x v="6"/>
+    <s v="Level Design"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Props"/>
-    <m/>
-    <x v="0"/>
-    <s v="3D Art"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="World"/>
+    <m/>
+    <x v="6"/>
+    <s v="Level Design"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Props"/>
-    <m/>
-    <x v="0"/>
-    <s v="3D Art"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="World"/>
+    <m/>
+    <x v="6"/>
+    <s v="Level Design"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Props"/>
-    <m/>
-    <x v="0"/>
-    <s v="3D Art"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="World"/>
+    <m/>
+    <x v="6"/>
+    <s v="Level Design"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="Props"/>
-    <m/>
-    <x v="0"/>
-    <s v="3D Art"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="World"/>
+    <m/>
+    <x v="6"/>
+    <s v="Level Design"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Props"/>
-    <m/>
-    <x v="0"/>
-    <s v="3D Art"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="World"/>
+    <m/>
+    <x v="6"/>
+    <s v="Level Design"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Props"/>
-    <m/>
-    <x v="0"/>
-    <s v="3D Art"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="World"/>
+    <m/>
+    <x v="6"/>
+    <s v="Level Design"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Props"/>
-    <m/>
-    <x v="0"/>
-    <s v="3D Art"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="World"/>
+    <m/>
+    <x v="6"/>
+    <s v="Level Design"/>
+    <m/>
+    <x v="3"/>
   </r>
   <r>
     <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Props"/>
-    <m/>
-    <x v="0"/>
-    <s v="3D Art"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Props"/>
-    <m/>
-    <x v="0"/>
-    <s v="3D Art"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Props"/>
-    <m/>
-    <x v="0"/>
-    <s v="3D Art"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="Props"/>
-    <m/>
-    <x v="0"/>
-    <s v="3D Art"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Puzzle"/>
-    <m/>
-    <x v="0"/>
+    <m/>
+    <s v="Zones"/>
+    <m/>
+    <x v="6"/>
     <s v="Code"/>
     <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Puzzle"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Puzzle"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <s v="0 - Must Have"/>
-    <s v="UI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="UI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="UI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="UI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Other"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="UI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Other"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="UI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Other"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="UI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Other"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="UI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="UI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="UI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="UI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="UI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Other"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="UI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Other"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="UI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Other"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="UI"/>
-    <m/>
-    <x v="0"/>
-    <s v="Other"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="2"/>
-    <s v="0 - Must Have"/>
-    <s v="World"/>
-    <m/>
-    <x v="0"/>
-    <s v="Level Design"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="World"/>
-    <m/>
-    <x v="0"/>
-    <s v="Level Design"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="World"/>
-    <m/>
-    <x v="0"/>
-    <s v="Level Design"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="World"/>
-    <m/>
-    <x v="0"/>
-    <s v="Level Design"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="World"/>
-    <m/>
-    <x v="0"/>
-    <s v="Level Design"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="World"/>
-    <m/>
-    <x v="0"/>
-    <s v="Level Design"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="World"/>
-    <m/>
-    <x v="0"/>
-    <s v="Level Design"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="World"/>
-    <m/>
-    <x v="0"/>
-    <s v="Level Design"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="World"/>
-    <m/>
-    <x v="0"/>
-    <s v="Level Design"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="World"/>
-    <m/>
-    <x v="0"/>
-    <s v="Level Design"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="1 - Should Have"/>
-    <s v="World"/>
-    <m/>
-    <x v="0"/>
-    <s v="Level Design"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="World"/>
-    <m/>
-    <x v="0"/>
-    <s v="Level Design"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="World"/>
-    <m/>
-    <x v="0"/>
-    <s v="Level Design"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="World"/>
-    <m/>
-    <x v="0"/>
-    <s v="Level Design"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="0 - Must Have"/>
-    <s v="World"/>
-    <m/>
-    <x v="0"/>
-    <s v="Level Design"/>
-    <m/>
-    <x v="0"/>
-  </r>
-  <r>
-    <x v="0"/>
-    <s v="2 - Could Have"/>
-    <s v="Zones"/>
-    <m/>
-    <x v="0"/>
-    <s v="Code"/>
-    <m/>
-    <x v="0"/>
+    <x v="3"/>
   </r>
 </pivotCacheRecords>
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Project Stats" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="5" compact="0" compactData="0">
-  <location ref="B3:F6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Project Stats" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="5" compact="0" compactData="0">
+  <location ref="B3:F12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField name="Completion" axis="axisCol" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
       <items count="4">
+        <item x="2"/>
         <item x="1"/>
-        <item x="2"/>
         <item x="0"/>
         <item t="default"/>
       </items>
@@ -2386,8 +2426,14 @@
     <pivotField name="EPIC" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
     <pivotField name="Task" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
     <pivotField name="Owner" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
-      <items count="2">
+      <items count="8">
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
         <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2398,9 +2444,27 @@
   <rowFields count="1">
     <field x="4"/>
   </rowFields>
-  <rowItems count="2">
+  <rowItems count="8">
     <i>
       <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
     </i>
     <i t="grand">
       <x/>
@@ -2431,24 +2495,34 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Project Stats 2" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="5" compact="0" compactData="0">
-  <location ref="H3:J6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Project Stats 2" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="5" compact="0" compactData="0">
+  <location ref="H3:N12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="8">
     <pivotField name="Completion" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
     <pivotField name="Priority" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
     <pivotField name="EPIC" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
     <pivotField name="Task" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
     <pivotField name="Owner" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
-      <items count="2">
+      <items count="8">
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
         <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField name="Type" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
     <pivotField name="Estimation (h)" dataField="1" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
     <pivotField name="Planned Week" axis="axisCol" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
-      <items count="2">
+      <items count="6">
+        <item x="2"/>
+        <item x="1"/>
         <item x="0"/>
+        <item x="4"/>
+        <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2456,9 +2530,27 @@
   <rowFields count="1">
     <field x="4"/>
   </rowFields>
-  <rowItems count="2">
+  <rowItems count="8">
     <i>
       <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
     </i>
     <i t="grand">
       <x/>
@@ -2467,9 +2559,21 @@
   <colFields count="1">
     <field x="7"/>
   </colFields>
-  <colItems count="2">
+  <colItems count="6">
     <i>
       <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
     </i>
     <i t="grand">
       <x/>
@@ -2483,14 +2587,14 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Project Stats 3" cacheId="20" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="5" compact="0" compactData="0">
-  <location ref="P3:R6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Project Stats 3" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0" dataCaption="" updatedVersion="5" compact="0" compactData="0">
+  <location ref="P3:U12" firstHeaderRow="1" firstDataRow="2" firstDataCol="1" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField name="Completion" axis="axisPage" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0">
       <items count="4">
         <item x="0"/>
+        <item h="1" x="2"/>
         <item h="1" x="1"/>
-        <item h="1" x="2"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2498,16 +2602,26 @@
     <pivotField name="EPIC" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
     <pivotField name="Task" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
     <pivotField name="Owner" axis="axisRow" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
-      <items count="2">
+      <items count="8">
+        <item x="2"/>
+        <item x="4"/>
+        <item x="5"/>
         <item x="0"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="6"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField name="Type" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
     <pivotField name="Estimation (h)" dataField="1" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0"/>
     <pivotField name="Planned Week" axis="axisCol" compact="0" outline="0" multipleItemSelectionAllowed="1" showAll="0" sortType="ascending">
-      <items count="2">
+      <items count="6">
+        <item x="2"/>
+        <item x="1"/>
         <item x="0"/>
+        <item x="4"/>
+        <item x="3"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2515,9 +2629,27 @@
   <rowFields count="1">
     <field x="4"/>
   </rowFields>
-  <rowItems count="2">
+  <rowItems count="8">
     <i>
       <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
     </i>
     <i t="grand">
       <x/>
@@ -2526,9 +2658,18 @@
   <colFields count="1">
     <field x="7"/>
   </colFields>
-  <colItems count="2">
+  <colItems count="5">
     <i>
-      <x/>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
     </i>
     <i t="grand">
       <x/>
@@ -2745,7 +2886,7 @@
   <dimension ref="B2:I1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="H26" sqref="H26"/>
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.625" defaultRowHeight="15" customHeight="1"/>
@@ -2762,16 +2903,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="23.25">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="2:9" ht="15.75">
       <c r="B3" s="1" t="s">
@@ -2837,7 +2978,7 @@
       <c r="F5" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H5" s="9"/>
@@ -2859,7 +3000,7 @@
       <c r="F6" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H6" s="9">
@@ -2883,7 +3024,7 @@
       <c r="F7" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H7" s="9"/>
@@ -2905,7 +3046,7 @@
       <c r="F8" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H8" s="9"/>
@@ -2927,7 +3068,7 @@
       <c r="F9" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H9" s="9">
@@ -2951,7 +3092,7 @@
       <c r="F10" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H10" s="9"/>
@@ -2973,7 +3114,7 @@
       <c r="F11" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H11" s="9">
@@ -2993,7 +3134,7 @@
         <v>105</v>
       </c>
       <c r="F12" s="15"/>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H12" s="9"/>
@@ -3009,7 +3150,7 @@
         <v>106</v>
       </c>
       <c r="F13" s="15"/>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H13" s="9"/>
@@ -3029,7 +3170,7 @@
       <c r="F14" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H14" s="9"/>
@@ -3051,8 +3192,8 @@
       <c r="F15" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="G15" s="9" t="s">
-        <v>47</v>
+      <c r="G15" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H15" s="9">
         <v>5</v>
@@ -3075,8 +3216,8 @@
       <c r="F16" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="G16" s="9" t="s">
-        <v>47</v>
+      <c r="G16" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H16" s="9">
         <v>5</v>
@@ -3099,8 +3240,8 @@
       <c r="F17" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="G17" s="9" t="s">
-        <v>47</v>
+      <c r="G17" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H17" s="9">
         <v>2</v>
@@ -3123,8 +3264,8 @@
       <c r="F18" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="G18" s="9" t="s">
-        <v>47</v>
+      <c r="G18" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H18" s="9"/>
       <c r="I18" s="16">
@@ -3145,8 +3286,8 @@
       <c r="F19" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="G19" s="9" t="s">
-        <v>47</v>
+      <c r="G19" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="16">
@@ -3167,8 +3308,8 @@
       <c r="F20" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="G20" s="9" t="s">
-        <v>47</v>
+      <c r="G20" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H20" s="9">
         <v>6</v>
@@ -3191,8 +3332,8 @@
       <c r="F21" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="G21" s="9" t="s">
-        <v>47</v>
+      <c r="G21" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="16">
@@ -3213,8 +3354,8 @@
       <c r="F22" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="G22" s="9" t="s">
-        <v>47</v>
+      <c r="G22" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H22" s="9"/>
       <c r="I22" s="16">
@@ -3225,26 +3366,40 @@
       <c r="B23" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="9"/>
+      <c r="C23" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="D23" s="9"/>
-      <c r="E23" s="20"/>
-      <c r="F23" s="15"/>
-      <c r="G23" s="9" t="s">
-        <v>47</v>
+      <c r="E23" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="F23" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="G23" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H23" s="9"/>
-      <c r="I23" s="16"/>
+      <c r="I23" s="16">
+        <v>3</v>
+      </c>
     </row>
     <row r="24" spans="2:9" ht="15.75" customHeight="1">
       <c r="B24" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="C24" s="9"/>
+      <c r="C24" s="9" t="s">
+        <v>12</v>
+      </c>
       <c r="D24" s="9"/>
-      <c r="E24" s="20"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="9" t="s">
-        <v>47</v>
+      <c r="E24" s="20" t="s">
+        <v>125</v>
+      </c>
+      <c r="F24" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="G24" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H24" s="9"/>
       <c r="I24" s="16"/>
@@ -3259,7 +3414,7 @@
       </c>
       <c r="E25" s="14"/>
       <c r="F25" s="15"/>
-      <c r="G25" s="9" t="s">
+      <c r="G25" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H25" s="9"/>
@@ -3275,8 +3430,8 @@
       </c>
       <c r="E26" s="20"/>
       <c r="F26" s="15"/>
-      <c r="G26" s="9" t="s">
-        <v>60</v>
+      <c r="G26" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H26" s="9"/>
       <c r="I26" s="16"/>
@@ -3291,8 +3446,8 @@
       </c>
       <c r="E27" s="20"/>
       <c r="F27" s="15"/>
-      <c r="G27" s="9" t="s">
-        <v>47</v>
+      <c r="G27" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H27" s="9"/>
       <c r="I27" s="16"/>
@@ -3307,8 +3462,8 @@
       </c>
       <c r="E28" s="20"/>
       <c r="F28" s="15"/>
-      <c r="G28" s="9" t="s">
-        <v>47</v>
+      <c r="G28" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H28" s="9"/>
       <c r="I28" s="16"/>
@@ -3323,8 +3478,8 @@
       </c>
       <c r="E29" s="20"/>
       <c r="F29" s="15"/>
-      <c r="G29" s="9" t="s">
-        <v>47</v>
+      <c r="G29" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H29" s="9"/>
       <c r="I29" s="16"/>
@@ -3339,8 +3494,8 @@
       </c>
       <c r="E30" s="20"/>
       <c r="F30" s="15"/>
-      <c r="G30" s="9" t="s">
-        <v>47</v>
+      <c r="G30" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="16"/>
@@ -3355,8 +3510,8 @@
       </c>
       <c r="E31" s="20"/>
       <c r="F31" s="23"/>
-      <c r="G31" s="9" t="s">
-        <v>60</v>
+      <c r="G31" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H31" s="9"/>
       <c r="I31" s="16"/>
@@ -3371,8 +3526,8 @@
       </c>
       <c r="E32" s="20"/>
       <c r="F32" s="23"/>
-      <c r="G32" s="9" t="s">
-        <v>60</v>
+      <c r="G32" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H32" s="9"/>
       <c r="I32" s="16"/>
@@ -3387,8 +3542,8 @@
       </c>
       <c r="E33" s="20"/>
       <c r="F33" s="23"/>
-      <c r="G33" s="9" t="s">
-        <v>60</v>
+      <c r="G33" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H33" s="9"/>
       <c r="I33" s="16"/>
@@ -3403,8 +3558,8 @@
       </c>
       <c r="E34" s="20"/>
       <c r="F34" s="23"/>
-      <c r="G34" s="9" t="s">
-        <v>60</v>
+      <c r="G34" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H34" s="9"/>
       <c r="I34" s="16"/>
@@ -3419,8 +3574,8 @@
       </c>
       <c r="E35" s="20"/>
       <c r="F35" s="23"/>
-      <c r="G35" s="9" t="s">
-        <v>60</v>
+      <c r="G35" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H35" s="9"/>
       <c r="I35" s="16"/>
@@ -3435,8 +3590,8 @@
       </c>
       <c r="E36" s="20"/>
       <c r="F36" s="23"/>
-      <c r="G36" s="9" t="s">
-        <v>60</v>
+      <c r="G36" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H36" s="9"/>
       <c r="I36" s="16"/>
@@ -3451,8 +3606,8 @@
       </c>
       <c r="E37" s="20"/>
       <c r="F37" s="23"/>
-      <c r="G37" s="9" t="s">
-        <v>60</v>
+      <c r="G37" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H37" s="9"/>
       <c r="I37" s="16"/>
@@ -3467,8 +3622,8 @@
       </c>
       <c r="E38" s="20"/>
       <c r="F38" s="15"/>
-      <c r="G38" s="9" t="s">
-        <v>60</v>
+      <c r="G38" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H38" s="9"/>
       <c r="I38" s="16"/>
@@ -3483,8 +3638,8 @@
       </c>
       <c r="E39" s="20"/>
       <c r="F39" s="15"/>
-      <c r="G39" s="9" t="s">
-        <v>60</v>
+      <c r="G39" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H39" s="9"/>
       <c r="I39" s="16"/>
@@ -3499,8 +3654,8 @@
       </c>
       <c r="E40" s="20"/>
       <c r="F40" s="15"/>
-      <c r="G40" s="9" t="s">
-        <v>60</v>
+      <c r="G40" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H40" s="9"/>
       <c r="I40" s="16"/>
@@ -3515,8 +3670,8 @@
       </c>
       <c r="E41" s="20"/>
       <c r="F41" s="15"/>
-      <c r="G41" s="9" t="s">
-        <v>60</v>
+      <c r="G41" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H41" s="9"/>
       <c r="I41" s="16"/>
@@ -3531,8 +3686,8 @@
       </c>
       <c r="E42" s="20"/>
       <c r="F42" s="23"/>
-      <c r="G42" s="9" t="s">
-        <v>47</v>
+      <c r="G42" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H42" s="9"/>
       <c r="I42" s="16"/>
@@ -3547,7 +3702,7 @@
       </c>
       <c r="E43" s="14"/>
       <c r="F43" s="15"/>
-      <c r="G43" s="9" t="s">
+      <c r="G43" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H43" s="9"/>
@@ -3563,7 +3718,7 @@
       </c>
       <c r="E44" s="14"/>
       <c r="F44" s="15"/>
-      <c r="G44" s="9" t="s">
+      <c r="G44" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H44" s="9"/>
@@ -3579,7 +3734,7 @@
       </c>
       <c r="E45" s="14"/>
       <c r="F45" s="23"/>
-      <c r="G45" s="9" t="s">
+      <c r="G45" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H45" s="9"/>
@@ -3595,7 +3750,7 @@
       </c>
       <c r="E46" s="14"/>
       <c r="F46" s="23"/>
-      <c r="G46" s="9" t="s">
+      <c r="G46" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H46" s="9"/>
@@ -3611,7 +3766,7 @@
       </c>
       <c r="E47" s="14"/>
       <c r="F47" s="23"/>
-      <c r="G47" s="9" t="s">
+      <c r="G47" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H47" s="9"/>
@@ -3627,7 +3782,7 @@
       </c>
       <c r="E48" s="14"/>
       <c r="F48" s="23"/>
-      <c r="G48" s="9" t="s">
+      <c r="G48" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H48" s="9"/>
@@ -3643,7 +3798,7 @@
       </c>
       <c r="E49" s="14"/>
       <c r="F49" s="23"/>
-      <c r="G49" s="9" t="s">
+      <c r="G49" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H49" s="9"/>
@@ -3659,7 +3814,7 @@
       </c>
       <c r="E50" s="14"/>
       <c r="F50" s="23"/>
-      <c r="G50" s="9" t="s">
+      <c r="G50" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H50" s="9"/>
@@ -3675,7 +3830,7 @@
       </c>
       <c r="E51" s="14"/>
       <c r="F51" s="23"/>
-      <c r="G51" s="9" t="s">
+      <c r="G51" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H51" s="9"/>
@@ -3691,7 +3846,7 @@
       </c>
       <c r="E52" s="14"/>
       <c r="F52" s="23"/>
-      <c r="G52" s="9" t="s">
+      <c r="G52" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H52" s="9"/>
@@ -3707,7 +3862,7 @@
       </c>
       <c r="E53" s="14"/>
       <c r="F53" s="23"/>
-      <c r="G53" s="9" t="s">
+      <c r="G53" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H53" s="9"/>
@@ -3723,7 +3878,7 @@
       </c>
       <c r="E54" s="14"/>
       <c r="F54" s="23"/>
-      <c r="G54" s="9" t="s">
+      <c r="G54" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H54" s="9"/>
@@ -3739,7 +3894,7 @@
       </c>
       <c r="E55" s="14"/>
       <c r="F55" s="23"/>
-      <c r="G55" s="9" t="s">
+      <c r="G55" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H55" s="9"/>
@@ -3755,7 +3910,7 @@
       </c>
       <c r="E56" s="14"/>
       <c r="F56" s="23"/>
-      <c r="G56" s="9" t="s">
+      <c r="G56" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H56" s="9"/>
@@ -3771,7 +3926,7 @@
       </c>
       <c r="E57" s="14"/>
       <c r="F57" s="23"/>
-      <c r="G57" s="9" t="s">
+      <c r="G57" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H57" s="9"/>
@@ -3787,8 +3942,8 @@
       </c>
       <c r="E58" s="20"/>
       <c r="F58" s="23"/>
-      <c r="G58" s="9" t="s">
-        <v>20</v>
+      <c r="G58" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H58" s="9"/>
       <c r="I58" s="16"/>
@@ -3803,8 +3958,8 @@
       </c>
       <c r="E59" s="20"/>
       <c r="F59" s="23"/>
-      <c r="G59" s="9" t="s">
-        <v>20</v>
+      <c r="G59" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H59" s="9"/>
       <c r="I59" s="16"/>
@@ -3819,8 +3974,8 @@
       </c>
       <c r="E60" s="20"/>
       <c r="F60" s="23"/>
-      <c r="G60" s="9" t="s">
-        <v>20</v>
+      <c r="G60" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H60" s="9"/>
       <c r="I60" s="16"/>
@@ -3835,8 +3990,8 @@
       </c>
       <c r="E61" s="20"/>
       <c r="F61" s="23"/>
-      <c r="G61" s="9" t="s">
-        <v>20</v>
+      <c r="G61" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H61" s="9"/>
       <c r="I61" s="16"/>
@@ -3851,8 +4006,8 @@
       </c>
       <c r="E62" s="20"/>
       <c r="F62" s="23"/>
-      <c r="G62" s="9" t="s">
-        <v>20</v>
+      <c r="G62" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H62" s="9"/>
       <c r="I62" s="16"/>
@@ -3867,8 +4022,8 @@
       </c>
       <c r="E63" s="20"/>
       <c r="F63" s="23"/>
-      <c r="G63" s="9" t="s">
-        <v>60</v>
+      <c r="G63" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H63" s="9"/>
       <c r="I63" s="16"/>
@@ -3883,8 +4038,8 @@
       </c>
       <c r="E64" s="20"/>
       <c r="F64" s="23"/>
-      <c r="G64" s="9" t="s">
-        <v>60</v>
+      <c r="G64" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H64" s="9"/>
       <c r="I64" s="16"/>
@@ -3899,8 +4054,8 @@
       </c>
       <c r="E65" s="20"/>
       <c r="F65" s="23"/>
-      <c r="G65" s="9" t="s">
-        <v>60</v>
+      <c r="G65" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H65" s="9"/>
       <c r="I65" s="16"/>
@@ -3915,8 +4070,8 @@
       </c>
       <c r="E66" s="20"/>
       <c r="F66" s="23"/>
-      <c r="G66" s="9" t="s">
-        <v>60</v>
+      <c r="G66" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H66" s="9"/>
       <c r="I66" s="16"/>
@@ -3931,8 +4086,8 @@
       </c>
       <c r="E67" s="20"/>
       <c r="F67" s="23"/>
-      <c r="G67" s="9" t="s">
-        <v>60</v>
+      <c r="G67" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H67" s="9"/>
       <c r="I67" s="16"/>
@@ -3947,8 +4102,8 @@
       </c>
       <c r="E68" s="20"/>
       <c r="F68" s="23"/>
-      <c r="G68" s="9" t="s">
-        <v>60</v>
+      <c r="G68" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H68" s="9"/>
       <c r="I68" s="16"/>
@@ -3963,8 +4118,8 @@
       </c>
       <c r="E69" s="20"/>
       <c r="F69" s="23"/>
-      <c r="G69" s="9" t="s">
-        <v>60</v>
+      <c r="G69" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H69" s="9"/>
       <c r="I69" s="16"/>
@@ -3979,8 +4134,8 @@
       </c>
       <c r="E70" s="24"/>
       <c r="F70" s="23"/>
-      <c r="G70" s="9" t="s">
-        <v>60</v>
+      <c r="G70" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H70" s="9"/>
       <c r="I70" s="16"/>
@@ -3995,8 +4150,8 @@
       </c>
       <c r="E71" s="24"/>
       <c r="F71" s="23"/>
-      <c r="G71" s="9" t="s">
-        <v>60</v>
+      <c r="G71" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H71" s="9"/>
       <c r="I71" s="16"/>
@@ -4011,8 +4166,8 @@
       </c>
       <c r="E72" s="24"/>
       <c r="F72" s="23"/>
-      <c r="G72" s="9" t="s">
-        <v>60</v>
+      <c r="G72" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H72" s="9"/>
       <c r="I72" s="16"/>
@@ -4027,8 +4182,8 @@
       </c>
       <c r="E73" s="24"/>
       <c r="F73" s="23"/>
-      <c r="G73" s="9" t="s">
-        <v>60</v>
+      <c r="G73" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H73" s="9"/>
       <c r="I73" s="16"/>
@@ -4043,8 +4198,8 @@
       </c>
       <c r="E74" s="20"/>
       <c r="F74" s="23"/>
-      <c r="G74" s="9" t="s">
-        <v>60</v>
+      <c r="G74" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H74" s="9"/>
       <c r="I74" s="16"/>
@@ -4059,8 +4214,8 @@
       </c>
       <c r="E75" s="20"/>
       <c r="F75" s="23"/>
-      <c r="G75" s="9" t="s">
-        <v>60</v>
+      <c r="G75" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H75" s="9"/>
       <c r="I75" s="16"/>
@@ -4075,8 +4230,8 @@
       </c>
       <c r="E76" s="20"/>
       <c r="F76" s="23"/>
-      <c r="G76" s="9" t="s">
-        <v>60</v>
+      <c r="G76" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H76" s="9"/>
       <c r="I76" s="16"/>
@@ -4091,8 +4246,8 @@
       </c>
       <c r="E77" s="20"/>
       <c r="F77" s="23"/>
-      <c r="G77" s="9" t="s">
-        <v>60</v>
+      <c r="G77" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H77" s="9"/>
       <c r="I77" s="16"/>
@@ -4107,8 +4262,8 @@
       </c>
       <c r="E78" s="20"/>
       <c r="F78" s="23"/>
-      <c r="G78" s="9" t="s">
-        <v>60</v>
+      <c r="G78" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H78" s="9"/>
       <c r="I78" s="16"/>
@@ -4123,7 +4278,7 @@
       </c>
       <c r="E79" s="14"/>
       <c r="F79" s="23"/>
-      <c r="G79" s="9" t="s">
+      <c r="G79" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H79" s="9"/>
@@ -4139,7 +4294,7 @@
       </c>
       <c r="E80" s="14"/>
       <c r="F80" s="23"/>
-      <c r="G80" s="9" t="s">
+      <c r="G80" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H80" s="9"/>
@@ -4155,7 +4310,7 @@
       </c>
       <c r="E81" s="14"/>
       <c r="F81" s="23"/>
-      <c r="G81" s="9" t="s">
+      <c r="G81" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H81" s="9"/>
@@ -4171,7 +4326,7 @@
       </c>
       <c r="E82" s="14"/>
       <c r="F82" s="23"/>
-      <c r="G82" s="9" t="s">
+      <c r="G82" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H82" s="9"/>
@@ -4187,7 +4342,7 @@
       </c>
       <c r="E83" s="14"/>
       <c r="F83" s="23"/>
-      <c r="G83" s="9" t="s">
+      <c r="G83" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H83" s="9"/>
@@ -4203,7 +4358,7 @@
       </c>
       <c r="E84" s="14"/>
       <c r="F84" s="23"/>
-      <c r="G84" s="9" t="s">
+      <c r="G84" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H84" s="9"/>
@@ -4219,8 +4374,8 @@
       </c>
       <c r="E85" s="20"/>
       <c r="F85" s="23"/>
-      <c r="G85" s="9" t="s">
-        <v>20</v>
+      <c r="G85" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H85" s="9"/>
       <c r="I85" s="16"/>
@@ -4235,8 +4390,8 @@
       </c>
       <c r="E86" s="20"/>
       <c r="F86" s="23"/>
-      <c r="G86" s="9" t="s">
-        <v>20</v>
+      <c r="G86" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H86" s="9"/>
       <c r="I86" s="16"/>
@@ -4251,8 +4406,8 @@
       </c>
       <c r="E87" s="20"/>
       <c r="F87" s="23"/>
-      <c r="G87" s="9" t="s">
-        <v>20</v>
+      <c r="G87" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H87" s="9"/>
       <c r="I87" s="16"/>
@@ -4267,8 +4422,8 @@
       </c>
       <c r="E88" s="20"/>
       <c r="F88" s="23"/>
-      <c r="G88" s="9" t="s">
-        <v>20</v>
+      <c r="G88" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H88" s="9"/>
       <c r="I88" s="16"/>
@@ -4283,7 +4438,7 @@
       </c>
       <c r="E89" s="14"/>
       <c r="F89" s="23"/>
-      <c r="G89" s="9" t="s">
+      <c r="G89" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H89" s="9"/>
@@ -4299,7 +4454,7 @@
       </c>
       <c r="E90" s="14"/>
       <c r="F90" s="23"/>
-      <c r="G90" s="9" t="s">
+      <c r="G90" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H90" s="9"/>
@@ -4315,7 +4470,7 @@
       </c>
       <c r="E91" s="14"/>
       <c r="F91" s="23"/>
-      <c r="G91" s="9" t="s">
+      <c r="G91" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H91" s="9"/>
@@ -4331,7 +4486,7 @@
       </c>
       <c r="E92" s="14"/>
       <c r="F92" s="23"/>
-      <c r="G92" s="9" t="s">
+      <c r="G92" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H92" s="9"/>
@@ -4347,8 +4502,8 @@
       </c>
       <c r="E93" s="20"/>
       <c r="F93" s="23"/>
-      <c r="G93" s="9" t="s">
-        <v>20</v>
+      <c r="G93" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H93" s="9"/>
       <c r="I93" s="16"/>
@@ -4363,8 +4518,8 @@
       </c>
       <c r="E94" s="20"/>
       <c r="F94" s="23"/>
-      <c r="G94" s="9" t="s">
-        <v>20</v>
+      <c r="G94" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H94" s="9"/>
       <c r="I94" s="16"/>
@@ -4379,8 +4534,8 @@
       </c>
       <c r="E95" s="20"/>
       <c r="F95" s="23"/>
-      <c r="G95" s="9" t="s">
-        <v>20</v>
+      <c r="G95" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H95" s="9"/>
       <c r="I95" s="16"/>
@@ -4395,8 +4550,8 @@
       </c>
       <c r="E96" s="20"/>
       <c r="F96" s="23"/>
-      <c r="G96" s="9" t="s">
-        <v>20</v>
+      <c r="G96" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H96" s="9"/>
       <c r="I96" s="16"/>
@@ -4411,8 +4566,8 @@
       </c>
       <c r="E97" s="20"/>
       <c r="F97" s="23"/>
-      <c r="G97" s="9" t="s">
-        <v>22</v>
+      <c r="G97" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H97" s="9"/>
       <c r="I97" s="16"/>
@@ -4427,8 +4582,8 @@
       </c>
       <c r="E98" s="20"/>
       <c r="F98" s="23"/>
-      <c r="G98" s="9" t="s">
-        <v>22</v>
+      <c r="G98" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H98" s="9"/>
       <c r="I98" s="16"/>
@@ -4443,8 +4598,8 @@
       </c>
       <c r="E99" s="20"/>
       <c r="F99" s="23"/>
-      <c r="G99" s="9" t="s">
-        <v>22</v>
+      <c r="G99" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H99" s="9"/>
       <c r="I99" s="16"/>
@@ -4459,8 +4614,8 @@
       </c>
       <c r="E100" s="20"/>
       <c r="F100" s="23"/>
-      <c r="G100" s="9" t="s">
-        <v>22</v>
+      <c r="G100" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H100" s="9"/>
       <c r="I100" s="16"/>
@@ -4475,8 +4630,8 @@
       </c>
       <c r="E101" s="20"/>
       <c r="F101" s="23"/>
-      <c r="G101" s="9" t="s">
-        <v>22</v>
+      <c r="G101" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H101" s="9"/>
       <c r="I101" s="16"/>
@@ -4491,8 +4646,8 @@
       </c>
       <c r="E102" s="20"/>
       <c r="F102" s="23"/>
-      <c r="G102" s="9" t="s">
-        <v>22</v>
+      <c r="G102" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H102" s="9"/>
       <c r="I102" s="16"/>
@@ -4507,8 +4662,8 @@
       </c>
       <c r="E103" s="20"/>
       <c r="F103" s="23"/>
-      <c r="G103" s="9" t="s">
-        <v>22</v>
+      <c r="G103" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H103" s="9"/>
       <c r="I103" s="16"/>
@@ -4523,8 +4678,8 @@
       </c>
       <c r="E104" s="20"/>
       <c r="F104" s="23"/>
-      <c r="G104" s="9" t="s">
-        <v>22</v>
+      <c r="G104" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H104" s="9"/>
       <c r="I104" s="16"/>
@@ -4539,8 +4694,8 @@
       </c>
       <c r="E105" s="20"/>
       <c r="F105" s="23"/>
-      <c r="G105" s="9" t="s">
-        <v>22</v>
+      <c r="G105" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H105" s="9"/>
       <c r="I105" s="16"/>
@@ -4555,8 +4710,8 @@
       </c>
       <c r="E106" s="20"/>
       <c r="F106" s="23"/>
-      <c r="G106" s="9" t="s">
-        <v>22</v>
+      <c r="G106" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H106" s="9"/>
       <c r="I106" s="16"/>
@@ -4571,8 +4726,8 @@
       </c>
       <c r="E107" s="20"/>
       <c r="F107" s="23"/>
-      <c r="G107" s="9" t="s">
-        <v>22</v>
+      <c r="G107" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H107" s="9"/>
       <c r="I107" s="16"/>
@@ -4587,8 +4742,8 @@
       </c>
       <c r="E108" s="20"/>
       <c r="F108" s="23"/>
-      <c r="G108" s="9" t="s">
-        <v>22</v>
+      <c r="G108" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H108" s="9"/>
       <c r="I108" s="16"/>
@@ -4603,8 +4758,8 @@
       </c>
       <c r="E109" s="20"/>
       <c r="F109" s="23"/>
-      <c r="G109" s="9" t="s">
-        <v>22</v>
+      <c r="G109" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H109" s="9"/>
       <c r="I109" s="16"/>
@@ -4619,8 +4774,8 @@
       </c>
       <c r="E110" s="20"/>
       <c r="F110" s="23"/>
-      <c r="G110" s="9" t="s">
-        <v>22</v>
+      <c r="G110" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H110" s="9"/>
       <c r="I110" s="16"/>
@@ -4635,8 +4790,8 @@
       </c>
       <c r="E111" s="20"/>
       <c r="F111" s="23"/>
-      <c r="G111" s="9" t="s">
-        <v>22</v>
+      <c r="G111" s="8" t="s">
+        <v>21</v>
       </c>
       <c r="H111" s="9"/>
       <c r="I111" s="16"/>
@@ -4651,7 +4806,7 @@
       </c>
       <c r="E112" s="14"/>
       <c r="F112" s="23"/>
-      <c r="G112" s="9" t="s">
+      <c r="G112" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H112" s="9"/>
@@ -5621,16 +5776,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="23.25">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="2:9" ht="15.75">
       <c r="B3" s="1" t="s">
@@ -8419,16 +8574,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:9" ht="23.25">
-      <c r="B2" s="48" t="s">
+      <c r="B2" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="50"/>
+      <c r="C2" s="64"/>
+      <c r="D2" s="64"/>
+      <c r="E2" s="64"/>
+      <c r="F2" s="64"/>
+      <c r="G2" s="64"/>
+      <c r="H2" s="64"/>
+      <c r="I2" s="65"/>
     </row>
     <row r="3" spans="2:9" ht="15.75">
       <c r="B3" s="1" t="s">
@@ -11523,277 +11678,416 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:22" ht="14.25">
-      <c r="P1" s="72" t="s">
+      <c r="P1" s="61" t="s">
         <v>1</v>
       </c>
-      <c r="Q1" s="73" t="s">
+      <c r="Q1" s="62" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="2" spans="2:22" ht="23.25">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="C2" s="52"/>
-      <c r="D2" s="52"/>
-      <c r="E2" s="52"/>
-      <c r="F2" s="53"/>
-      <c r="H2" s="51" t="s">
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="68"/>
+      <c r="H2" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="52"/>
-      <c r="J2" s="52"/>
-      <c r="K2" s="52"/>
-      <c r="L2" s="52"/>
-      <c r="M2" s="52"/>
-      <c r="N2" s="53"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="52"/>
-      <c r="R2" s="52"/>
-      <c r="S2" s="52"/>
-      <c r="T2" s="52"/>
-      <c r="U2" s="52"/>
-      <c r="V2" s="53"/>
+      <c r="I2" s="67"/>
+      <c r="J2" s="67"/>
+      <c r="K2" s="67"/>
+      <c r="L2" s="67"/>
+      <c r="M2" s="67"/>
+      <c r="N2" s="68"/>
+      <c r="P2" s="66"/>
+      <c r="Q2" s="67"/>
+      <c r="R2" s="67"/>
+      <c r="S2" s="67"/>
+      <c r="T2" s="67"/>
+      <c r="U2" s="67"/>
+      <c r="V2" s="68"/>
     </row>
     <row r="3" spans="2:22" ht="14.25">
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="48" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="60"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="61"/>
-      <c r="H3" s="59" t="s">
+      <c r="D3" s="49"/>
+      <c r="E3" s="49"/>
+      <c r="F3" s="50"/>
+      <c r="H3" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="I3" s="59" t="s">
+      <c r="I3" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="J3" s="61"/>
-      <c r="P3" s="59" t="s">
+      <c r="J3" s="49"/>
+      <c r="K3" s="49"/>
+      <c r="L3" s="49"/>
+      <c r="M3" s="49"/>
+      <c r="N3" s="50"/>
+      <c r="P3" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="Q3" s="59" t="s">
+      <c r="Q3" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="R3" s="61"/>
-    </row>
-    <row r="4" spans="2:22">
-      <c r="B4" s="59" t="s">
+      <c r="R3" s="49"/>
+      <c r="S3" s="49"/>
+      <c r="T3" s="49"/>
+      <c r="U3" s="50"/>
+    </row>
+    <row r="4" spans="2:22" ht="14.25">
+      <c r="B4" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="63" t="s">
+      <c r="D4" s="52" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="63" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" s="64" t="s">
+      <c r="E4" s="52" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="H4" s="59" t="s">
+      <c r="H4" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="I4" s="62" t="s">
+      <c r="I4" s="51">
+        <v>3</v>
+      </c>
+      <c r="J4" s="52">
+        <v>4</v>
+      </c>
+      <c r="K4" s="52">
+        <v>6</v>
+      </c>
+      <c r="L4" s="52">
+        <v>10</v>
+      </c>
+      <c r="M4" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="J4" s="64" t="s">
+      <c r="N4" s="53" t="s">
         <v>86</v>
       </c>
-      <c r="M4" s="15"/>
-      <c r="P4" s="59" t="s">
+      <c r="P4" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="Q4" s="62" t="s">
+      <c r="Q4" s="51">
+        <v>4</v>
+      </c>
+      <c r="R4" s="52">
+        <v>6</v>
+      </c>
+      <c r="S4" s="52">
+        <v>10</v>
+      </c>
+      <c r="T4" s="52" t="s">
         <v>98</v>
       </c>
-      <c r="R4" s="64" t="s">
+      <c r="U4" s="53" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="5" spans="2:22">
-      <c r="B5" s="62" t="s">
+      <c r="B5" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="C5" s="54"/>
+      <c r="D5" s="55">
+        <v>2</v>
+      </c>
+      <c r="E5" s="55"/>
+      <c r="F5" s="56">
+        <v>2</v>
+      </c>
+      <c r="H5" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="I5" s="54">
+        <v>2</v>
+      </c>
+      <c r="J5" s="55"/>
+      <c r="K5" s="55"/>
+      <c r="L5" s="55"/>
+      <c r="M5" s="55"/>
+      <c r="N5" s="56">
+        <v>2</v>
+      </c>
+      <c r="P5" s="51" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q5" s="54"/>
+      <c r="R5" s="55"/>
+      <c r="S5" s="55"/>
+      <c r="T5" s="55"/>
+      <c r="U5" s="56"/>
+      <c r="V5" s="25"/>
+    </row>
+    <row r="6" spans="2:22">
+      <c r="B6" s="74" t="s">
+        <v>122</v>
+      </c>
+      <c r="C6" s="75"/>
+      <c r="D6" s="76"/>
+      <c r="E6" s="76">
+        <v>24</v>
+      </c>
+      <c r="F6" s="77">
+        <v>24</v>
+      </c>
+      <c r="H6" s="74" t="s">
+        <v>122</v>
+      </c>
+      <c r="I6" s="75"/>
+      <c r="J6" s="76">
+        <v>24</v>
+      </c>
+      <c r="K6" s="76"/>
+      <c r="L6" s="76"/>
+      <c r="M6" s="76"/>
+      <c r="N6" s="77">
+        <v>24</v>
+      </c>
+      <c r="P6" s="74" t="s">
+        <v>122</v>
+      </c>
+      <c r="Q6" s="75">
+        <v>24</v>
+      </c>
+      <c r="R6" s="76"/>
+      <c r="S6" s="76"/>
+      <c r="T6" s="76"/>
+      <c r="U6" s="77">
+        <v>24</v>
+      </c>
+      <c r="V6" s="25"/>
+    </row>
+    <row r="7" spans="2:22">
+      <c r="B7" s="74" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="75"/>
+      <c r="D7" s="76">
+        <v>10</v>
+      </c>
+      <c r="E7" s="76"/>
+      <c r="F7" s="77">
+        <v>10</v>
+      </c>
+      <c r="H7" s="74" t="s">
+        <v>123</v>
+      </c>
+      <c r="I7" s="75">
+        <v>10</v>
+      </c>
+      <c r="J7" s="76"/>
+      <c r="K7" s="76"/>
+      <c r="L7" s="76"/>
+      <c r="M7" s="76"/>
+      <c r="N7" s="77">
+        <v>10</v>
+      </c>
+      <c r="P7" s="74" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q7" s="75"/>
+      <c r="R7" s="76"/>
+      <c r="S7" s="76"/>
+      <c r="T7" s="76"/>
+      <c r="U7" s="77"/>
+      <c r="V7" s="25"/>
+    </row>
+    <row r="8" spans="2:22">
+      <c r="B8" s="74" t="s">
+        <v>118</v>
+      </c>
+      <c r="C8" s="75"/>
+      <c r="D8" s="76"/>
+      <c r="E8" s="76">
+        <v>28</v>
+      </c>
+      <c r="F8" s="77">
+        <v>28</v>
+      </c>
+      <c r="H8" s="74" t="s">
+        <v>118</v>
+      </c>
+      <c r="I8" s="75"/>
+      <c r="J8" s="76">
+        <v>6</v>
+      </c>
+      <c r="K8" s="76">
+        <v>22</v>
+      </c>
+      <c r="L8" s="76"/>
+      <c r="M8" s="76"/>
+      <c r="N8" s="77">
+        <v>28</v>
+      </c>
+      <c r="P8" s="74" t="s">
+        <v>118</v>
+      </c>
+      <c r="Q8" s="75">
+        <v>6</v>
+      </c>
+      <c r="R8" s="76">
+        <v>22</v>
+      </c>
+      <c r="S8" s="76"/>
+      <c r="T8" s="76"/>
+      <c r="U8" s="77">
+        <v>28</v>
+      </c>
+      <c r="V8" s="25"/>
+    </row>
+    <row r="9" spans="2:22">
+      <c r="B9" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="C9" s="75"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76">
+        <v>6</v>
+      </c>
+      <c r="F9" s="77">
+        <v>6</v>
+      </c>
+      <c r="H9" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="I9" s="75"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="76">
+        <v>6</v>
+      </c>
+      <c r="L9" s="76"/>
+      <c r="M9" s="76"/>
+      <c r="N9" s="77">
+        <v>6</v>
+      </c>
+      <c r="P9" s="74" t="s">
+        <v>119</v>
+      </c>
+      <c r="Q9" s="75"/>
+      <c r="R9" s="76">
+        <v>6</v>
+      </c>
+      <c r="S9" s="76"/>
+      <c r="T9" s="76"/>
+      <c r="U9" s="77">
+        <v>6</v>
+      </c>
+      <c r="V9" s="25"/>
+    </row>
+    <row r="10" spans="2:22">
+      <c r="B10" s="74" t="s">
+        <v>121</v>
+      </c>
+      <c r="C10" s="75"/>
+      <c r="D10" s="76"/>
+      <c r="E10" s="76"/>
+      <c r="F10" s="77"/>
+      <c r="H10" s="74" t="s">
+        <v>121</v>
+      </c>
+      <c r="I10" s="75"/>
+      <c r="J10" s="76"/>
+      <c r="K10" s="76"/>
+      <c r="L10" s="76"/>
+      <c r="M10" s="76"/>
+      <c r="N10" s="77"/>
+      <c r="P10" s="74" t="s">
+        <v>121</v>
+      </c>
+      <c r="Q10" s="75"/>
+      <c r="R10" s="76"/>
+      <c r="S10" s="76"/>
+      <c r="T10" s="76"/>
+      <c r="U10" s="77"/>
+      <c r="V10" s="25"/>
+    </row>
+    <row r="11" spans="2:22">
+      <c r="B11" s="74" t="s">
         <v>98</v>
       </c>
-      <c r="C5" s="65"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="67"/>
-      <c r="H5" s="62" t="s">
+      <c r="C11" s="75"/>
+      <c r="D11" s="76"/>
+      <c r="E11" s="76"/>
+      <c r="F11" s="77"/>
+      <c r="H11" s="74" t="s">
         <v>98</v>
       </c>
-      <c r="I5" s="65"/>
-      <c r="J5" s="67"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25"/>
-      <c r="P5" s="62" t="s">
+      <c r="I11" s="75"/>
+      <c r="J11" s="76"/>
+      <c r="K11" s="76"/>
+      <c r="L11" s="76"/>
+      <c r="M11" s="76"/>
+      <c r="N11" s="77"/>
+      <c r="P11" s="74" t="s">
         <v>98</v>
       </c>
-      <c r="Q5" s="65"/>
-      <c r="R5" s="67"/>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
-      <c r="V5" s="25"/>
-    </row>
-    <row r="6" spans="2:22">
-      <c r="B6" s="68" t="s">
+      <c r="Q11" s="75"/>
+      <c r="R11" s="76"/>
+      <c r="S11" s="76"/>
+      <c r="T11" s="76"/>
+      <c r="U11" s="77"/>
+      <c r="V11" s="25"/>
+    </row>
+    <row r="12" spans="2:22">
+      <c r="B12" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="69"/>
-      <c r="D6" s="70"/>
-      <c r="E6" s="70"/>
-      <c r="F6" s="71"/>
-      <c r="H6" s="68" t="s">
+      <c r="C12" s="58"/>
+      <c r="D12" s="59">
+        <v>12</v>
+      </c>
+      <c r="E12" s="59">
+        <v>58</v>
+      </c>
+      <c r="F12" s="60">
+        <v>70</v>
+      </c>
+      <c r="H12" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="I6" s="69"/>
-      <c r="J6" s="71"/>
-      <c r="K6" s="25"/>
-      <c r="L6" s="25"/>
-      <c r="M6" s="25"/>
-      <c r="N6" s="25"/>
-      <c r="P6" s="68" t="s">
+      <c r="I12" s="58">
+        <v>12</v>
+      </c>
+      <c r="J12" s="59">
+        <v>30</v>
+      </c>
+      <c r="K12" s="59">
+        <v>28</v>
+      </c>
+      <c r="L12" s="59"/>
+      <c r="M12" s="59"/>
+      <c r="N12" s="60">
+        <v>70</v>
+      </c>
+      <c r="P12" s="57" t="s">
         <v>86</v>
       </c>
-      <c r="Q6" s="69"/>
-      <c r="R6" s="71"/>
-      <c r="S6" s="25"/>
-      <c r="T6" s="25"/>
-      <c r="U6" s="25"/>
-      <c r="V6" s="25"/>
-    </row>
-    <row r="7" spans="2:22">
-      <c r="B7" s="42"/>
-      <c r="C7" s="25"/>
-      <c r="D7" s="25"/>
-      <c r="E7" s="25"/>
-      <c r="F7" s="25"/>
-      <c r="H7" s="42"/>
-      <c r="I7" s="25"/>
-      <c r="J7" s="25"/>
-      <c r="K7" s="25"/>
-      <c r="L7" s="25"/>
-      <c r="M7" s="25"/>
-      <c r="N7" s="25"/>
-      <c r="P7" s="42"/>
-      <c r="Q7" s="25"/>
-      <c r="R7" s="25"/>
-      <c r="S7" s="25"/>
-      <c r="T7" s="25"/>
-      <c r="U7" s="25"/>
-      <c r="V7" s="25"/>
-    </row>
-    <row r="8" spans="2:22">
-      <c r="B8" s="42"/>
-      <c r="C8" s="25"/>
-      <c r="D8" s="25"/>
-      <c r="E8" s="25"/>
-      <c r="F8" s="25"/>
-      <c r="H8" s="42"/>
-      <c r="I8" s="25"/>
-      <c r="J8" s="25"/>
-      <c r="K8" s="25"/>
-      <c r="L8" s="25"/>
-      <c r="M8" s="25"/>
-      <c r="N8" s="25"/>
-      <c r="P8" s="42"/>
-      <c r="Q8" s="25"/>
-      <c r="R8" s="25"/>
-      <c r="S8" s="25"/>
-      <c r="T8" s="25"/>
-      <c r="U8" s="25"/>
-      <c r="V8" s="25"/>
-    </row>
-    <row r="9" spans="2:22">
-      <c r="B9" s="42"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="H9" s="42"/>
-      <c r="I9" s="25"/>
-      <c r="J9" s="25"/>
-      <c r="K9" s="25"/>
-      <c r="L9" s="25"/>
-      <c r="M9" s="25"/>
-      <c r="N9" s="25"/>
-      <c r="P9" s="42"/>
-      <c r="Q9" s="25"/>
-      <c r="R9" s="25"/>
-      <c r="S9" s="25"/>
-      <c r="T9" s="25"/>
-      <c r="U9" s="25"/>
-      <c r="V9" s="25"/>
-    </row>
-    <row r="10" spans="2:22">
-      <c r="B10" s="42"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="H10" s="42"/>
-      <c r="I10" s="25"/>
-      <c r="J10" s="25"/>
-      <c r="K10" s="25"/>
-      <c r="L10" s="25"/>
-      <c r="M10" s="25"/>
-      <c r="N10" s="25"/>
-      <c r="P10" s="42"/>
-      <c r="Q10" s="25"/>
-      <c r="R10" s="25"/>
-      <c r="S10" s="25"/>
-      <c r="T10" s="25"/>
-      <c r="U10" s="25"/>
-      <c r="V10" s="25"/>
-    </row>
-    <row r="11" spans="2:22">
-      <c r="B11" s="42"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
-      <c r="H11" s="42"/>
-      <c r="I11" s="25"/>
-      <c r="J11" s="25"/>
-      <c r="K11" s="25"/>
-      <c r="L11" s="25"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="25"/>
-      <c r="P11" s="42"/>
-      <c r="Q11" s="25"/>
-      <c r="R11" s="25"/>
-      <c r="S11" s="25"/>
-      <c r="T11" s="25"/>
-      <c r="U11" s="25"/>
-      <c r="V11" s="25"/>
-    </row>
-    <row r="12" spans="2:22">
-      <c r="B12" s="42"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="H12" s="42"/>
-      <c r="I12" s="25"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="25"/>
-      <c r="N12" s="25"/>
-      <c r="P12" s="42"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="25"/>
-      <c r="S12" s="25"/>
-      <c r="T12" s="25"/>
-      <c r="U12" s="25"/>
+      <c r="Q12" s="58">
+        <v>30</v>
+      </c>
+      <c r="R12" s="59">
+        <v>28</v>
+      </c>
+      <c r="S12" s="59"/>
+      <c r="T12" s="59"/>
+      <c r="U12" s="60">
+        <v>58</v>
+      </c>
       <c r="V12" s="25"/>
     </row>
     <row r="13" spans="2:22">
@@ -11818,13 +12112,13 @@
       <c r="V13" s="25"/>
     </row>
     <row r="17" spans="2:6" ht="23.25">
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="53"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="67"/>
+      <c r="E17" s="67"/>
+      <c r="F17" s="68"/>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="43" t="s">
@@ -11834,10 +12128,10 @@
       <c r="D18" s="44">
         <v>14</v>
       </c>
-      <c r="E18" s="55" t="s">
+      <c r="E18" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="F18" s="56"/>
+      <c r="F18" s="70"/>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" s="43" t="s">
@@ -11847,10 +12141,10 @@
       <c r="D19" s="44">
         <v>16</v>
       </c>
-      <c r="E19" s="55" t="s">
+      <c r="E19" s="69" t="s">
         <v>91</v>
       </c>
-      <c r="F19" s="56"/>
+      <c r="F19" s="70"/>
     </row>
     <row r="20" spans="2:6">
       <c r="B20" s="43" t="s">
@@ -11860,10 +12154,10 @@
       <c r="D20" s="44">
         <v>7</v>
       </c>
-      <c r="E20" s="57" t="s">
+      <c r="E20" s="71" t="s">
         <v>93</v>
       </c>
-      <c r="F20" s="58"/>
+      <c r="F20" s="72"/>
     </row>
     <row r="21" spans="2:6" ht="15.75" customHeight="1">
       <c r="B21" s="45"/>
@@ -11881,13 +12175,13 @@
     <row r="23" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="24" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="25" spans="2:6" ht="15.75" customHeight="1">
-      <c r="B25" s="51" t="s">
+      <c r="B25" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="52"/>
-      <c r="D25" s="52"/>
-      <c r="E25" s="52"/>
-      <c r="F25" s="53"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="68"/>
     </row>
     <row r="26" spans="2:6" ht="15.75" customHeight="1">
       <c r="B26" s="43" t="s">
@@ -11895,11 +12189,11 @@
       </c>
       <c r="C26" s="43"/>
       <c r="D26" s="43"/>
-      <c r="E26" s="54">
+      <c r="E26" s="73">
         <f>GETPIVOTDATA("Estimation (h)",$B$3)/D21</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="50"/>
+        <v>4.4642857142857144E-2</v>
+      </c>
+      <c r="F26" s="65"/>
     </row>
     <row r="27" spans="2:6" ht="15.75" customHeight="1">
       <c r="B27" s="43" t="s">
@@ -11907,11 +12201,11 @@
       </c>
       <c r="C27" s="43"/>
       <c r="D27" s="43"/>
-      <c r="E27" s="54" t="e">
+      <c r="E27" s="73">
         <f>GETPIVOTDATA("Estimation (h)",$B$3,"Completion","Done")/GETPIVOTDATA("Estimation (h)",$B$3)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F27" s="50"/>
+        <v>0</v>
+      </c>
+      <c r="F27" s="65"/>
     </row>
     <row r="28" spans="2:6" ht="15.75" customHeight="1"/>
     <row r="29" spans="2:6" ht="15.75" customHeight="1"/>
@@ -12888,37 +13182,17 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B25:F25"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="B2:F2"/>
+    <mergeCell ref="H2:N2"/>
     <mergeCell ref="P2:V2"/>
     <mergeCell ref="B17:F17"/>
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="E19:F19"/>
     <mergeCell ref="E20:F20"/>
-    <mergeCell ref="B25:F25"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="B2:F2"/>
-    <mergeCell ref="H2:N2"/>
   </mergeCells>
-  <conditionalFormatting sqref="I7:L12 K5:L6">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
-      <formula>$D$19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7:L12 K5:L6">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>$D$19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I7:L12 K5:L6">
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="lessThan">
-      <formula>$D$19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Q7:T12 S5:T6">
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
-      <formula>0</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
 </worksheet>

</xml_diff>